<commit_message>
well it's kind of working
we need to do some fine tuning
</commit_message>
<xml_diff>
--- a/WGUPS Distance Table.xlsx
+++ b/WGUPS Distance Table.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -20,13 +20,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="55">
   <si>
     <t xml:space="preserve">DISTANCE BETWEEN HUBS IN MILES</t>
   </si>
   <si>
     <t xml:space="preserve">Western Governors University
-4001 South 700 East</t>
+4001 South 700 East, 
+Salt Lake City, UT 84107</t>
   </si>
   <si>
     <t xml:space="preserve">International Peace Gardens
@@ -133,10 +134,6 @@
  6351 South 900 East</t>
   </si>
   <si>
-    <t xml:space="preserve">Western Governors University
-4001 South 700 East </t>
-  </si>
-  <si>
     <t xml:space="preserve"> HUB</t>
   </si>
   <si>
@@ -232,7 +229,7 @@
 (84118)</t>
   </si>
   <si>
-    <t xml:space="preserve"> 5383 S 900 East #104
+    <t xml:space="preserve"> 5383 S 900 E
 (84117)</t>
   </si>
   <si>
@@ -608,6 +605,49 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>883800</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>60840</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>190080</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>230400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="0" name="Picture 2" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId1"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2230560" y="60840"/>
+          <a:ext cx="4624560" cy="415800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
   <a:themeElements>
@@ -787,8 +827,8 @@
   </sheetPr>
   <dimension ref="A1:AC1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B26" activeCellId="0" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.25" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -886,12 +926,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>28</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>29</v>
       </c>
       <c r="C2" s="9" t="n">
         <v>0</v>
@@ -928,7 +968,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C3" s="13" t="n">
         <v>7.2</v>
@@ -967,7 +1007,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C4" s="13" t="n">
         <v>3.8</v>
@@ -1008,7 +1048,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C5" s="13" t="n">
         <v>11</v>
@@ -1051,7 +1091,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C6" s="13" t="n">
         <v>2.2</v>
@@ -1096,7 +1136,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C7" s="13" t="n">
         <v>3.5</v>
@@ -1143,7 +1183,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C8" s="13" t="n">
         <v>10.9</v>
@@ -1192,7 +1232,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C9" s="13" t="n">
         <v>8.6</v>
@@ -1243,7 +1283,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C10" s="13" t="n">
         <v>7.6</v>
@@ -1296,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C11" s="13" t="n">
         <v>2.8</v>
@@ -1351,7 +1391,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C12" s="13" t="n">
         <v>6.4</v>
@@ -1408,7 +1448,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C13" s="13" t="n">
         <v>3.2</v>
@@ -1467,7 +1507,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C14" s="13" t="n">
         <v>7.6</v>
@@ -1528,7 +1568,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C15" s="13" t="n">
         <v>5.2</v>
@@ -1591,7 +1631,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C16" s="13" t="n">
         <v>4.4</v>
@@ -1656,7 +1696,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C17" s="13" t="n">
         <v>3.66112816434</v>
@@ -1723,7 +1763,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C18" s="13" t="n">
         <v>7.6</v>
@@ -1792,7 +1832,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C19" s="13" t="n">
         <v>2</v>
@@ -1863,7 +1903,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C20" s="13" t="n">
         <v>3.6</v>
@@ -1936,7 +1976,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C21" s="13" t="n">
         <v>6.5</v>
@@ -2011,7 +2051,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C22" s="13" t="n">
         <v>1.9</v>
@@ -2088,7 +2128,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C23" s="13" t="n">
         <v>3.4</v>
@@ -2167,7 +2207,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C24" s="13" t="n">
         <v>2.4</v>
@@ -2248,7 +2288,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C25" s="13" t="n">
         <v>6.4</v>
@@ -2331,7 +2371,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C26" s="13" t="n">
         <v>2.4</v>
@@ -2416,7 +2456,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C27" s="13" t="n">
         <v>5</v>
@@ -2503,7 +2543,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="17" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C28" s="18" t="n">
         <v>3.6</v>
@@ -2602,6 +2642,7 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>